<commit_message>
se suben los catalogos de los productos
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE672C7-7718-4431-9886-77F7B91A7745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B2F5D5E-7D5D-44BC-827A-931DC3FFB20F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{1E4C5145-BF0C-4FAE-8F34-669A9680EFA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{1E4C5145-BF0C-4FAE-8F34-669A9680EFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2 " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Actividades back End Administrador</t>
   </si>
@@ -76,6 +78,45 @@
   </si>
   <si>
     <t>A-B de Facturacion</t>
+  </si>
+  <si>
+    <t>1.-Antes de iniciar el modulo se debe configurar por estación , es decir que se debe identificar si es la primera vez que se abre  abrir un modal y configurar que numero de estación y guardarlo se me ocurre en el web.config</t>
+  </si>
+  <si>
+    <t>2.-Se debe de poder guardar una compra, sin afectar inventario ni nada solo guardar una compra por si después desean venderla.</t>
+  </si>
+  <si>
+    <t>3.- de debe poder editar una compra aun que esta ya este finalizada (debemos pensar la forma de regresar producto al inventario o a ese venta agregar producto y marcar la salida de inventario pero solo afectar el inventario del producto que se esta agregando.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.- En el modulo de ventas es importante tener en cuenta  que dependiendo de la cantidad del producto se aplica un precio y si el tipo de cliente es diferente a cliente general se aplica un ajuste al total de la venta. Esta por definirse el criterio de las 12 piezas el cual consiste en asignar un precio si el cliente lleva 12 piezas aunque no sea del mismo producto </t>
+  </si>
+  <si>
+    <t>5.- debe poder buscar un producto y conocer sus distintos tipo de precios</t>
+  </si>
+  <si>
+    <t>6.- Adicionar un modulo para configurar los rangos de precios</t>
+  </si>
+  <si>
+    <t>7.-Adicionar un modulo para cargar el porcentaje de descuento dependiendo el tipo de cliente</t>
+  </si>
+  <si>
+    <t>8.- Se debe realizar la facturacion al finalizar una compra  o despues de realizarla cuando se ven en el datatables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividades </t>
+  </si>
+  <si>
+    <t>9.-Agregar en el apartado de productos  un combo para seleccionar claveProdServ con base al catalogo FactCatClaveProdServicio</t>
+  </si>
+  <si>
+    <t>10.-agregar en el apartado de productos un combo para seleccionar claveUnidadSaT con base al catalofo FactCatClaveUnidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.- Generar ticket con la venta pensar que es un ticker como el de cualquier tienda chico no tamaño carta o algo asi como el que hizo blanquita para remesas </t>
+  </si>
+  <si>
+    <t>12.-Agregar modulo para agregar estaciones por punto de venta (Seleccionar Sucursal , despues punto de venta , y ahí agregar estacion)</t>
   </si>
 </sst>
 </file>
@@ -444,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFBBFC2-08B2-4254-AA2E-2CFF539BB5BE}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -540,4 +581,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B05468-98B6-4304-965F-940D000129DA}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se agregan campos de facturacion a vista de productos
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B2F5D5E-7D5D-44BC-827A-931DC3FFB20F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{1E4C5145-BF0C-4FAE-8F34-669A9680EFA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2 " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,15 +139,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,17 +167,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFBBFC2-08B2-4254-AA2E-2CFF539BB5BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -496,10 +525,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -551,7 +580,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -559,19 +588,19 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -584,84 +613,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B05468-98B6-4304-965F-940D000129DA}">
-  <dimension ref="A1:A13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="134.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se corrijen detalles de la vista de descuentos
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -159,21 +159,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -186,16 +177,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,10 +516,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -580,7 +571,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -588,19 +579,19 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -617,7 +608,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +653,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -672,12 +663,12 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agregan funciones de consulta de rangos de precios para los prodcctos
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -180,14 +180,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,10 +516,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -571,7 +571,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -579,19 +579,19 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -608,7 +608,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,17 +638,17 @@
       </c>
     </row>
     <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega el ticket a la venta
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FAD4A3-8B67-4495-8BE6-001BB8049440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2 " sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -120,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -502,7 +505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -604,11 +607,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +676,7 @@
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se marcan las actividades terminadas
</commit_message>
<xml_diff>
--- a/Analisis/Actividades.xlsx
+++ b/Analisis/Actividades.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FFAD18-9D5D-4023-8C54-58CB14A80D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +159,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,14 +193,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -516,10 +535,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -571,7 +590,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -579,19 +598,19 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -604,11 +623,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,17 +647,17 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -658,7 +677,7 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>